<commit_message>
add some problems of algorithm
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16494FE5-AC94-954E-BB96-2EF5F6B274C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B62900-ECE7-324D-89B6-DE2ABFE22B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20260" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
+    <workbookView xWindow="-27960" yWindow="3280" windowWidth="27960" windowHeight="17500" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$120</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="168">
   <si>
     <t>查找</t>
   </si>
@@ -526,6 +526,21 @@
   </si>
   <si>
     <t>字典树</t>
+  </si>
+  <si>
+    <t>105. 从前序与中序遍历序列构造二叉树</t>
+  </si>
+  <si>
+    <t>1143. 最长公共子序列</t>
+  </si>
+  <si>
+    <t>779. 第K个语法符号</t>
+  </si>
+  <si>
+    <t>位运算</t>
+  </si>
+  <si>
+    <t>2. 两数相加</t>
   </si>
 </sst>
 </file>
@@ -911,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}">
   <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="E115" sqref="E115"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2569,11 +2584,67 @@
         <v>5</v>
       </c>
     </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>119</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C118" t="s">
+        <v>50</v>
+      </c>
+      <c r="D118" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>120</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C119" t="s">
+        <v>14</v>
+      </c>
+      <c r="D119" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>121</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C120" t="s">
+        <v>166</v>
+      </c>
+      <c r="D120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>122</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C121" t="s">
+        <v>29</v>
+      </c>
+      <c r="D121" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D122" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D107" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}"/>
+  <autoFilter ref="A1:D120" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}"/>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" display="https://leetcode-cn.com/problems/delete-node-in-a-bst/" xr:uid="{905A4F28-94AF-E844-9890-0E957A75B3F3}"/>
     <hyperlink ref="B7" r:id="rId2" display="https://leetcode-cn.com/problems/kth-largest-element-in-an-array/" xr:uid="{F03E5809-027F-874F-ABCB-F9502E0418CD}"/>
@@ -2688,6 +2759,7 @@
     <hyperlink ref="B114" r:id="rId111" xr:uid="{6039090F-359F-5448-927D-AFAC478A96FA}"/>
     <hyperlink ref="B116" r:id="rId112" xr:uid="{CCB20CB5-2063-F042-842E-3DF1AACB70D8}"/>
     <hyperlink ref="B117" r:id="rId113" xr:uid="{B1355D50-FC41-944A-BDE7-7A26E99DFB3D}"/>
+    <hyperlink ref="B118" r:id="rId114" xr:uid="{ECF58827-D886-5544-8231-4C6D8F80D614}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add some problems of algorithms about stack
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B62900-ECE7-324D-89B6-DE2ABFE22B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40FB5ED-084D-3548-A772-9047753FF271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27960" yWindow="3280" windowWidth="27960" windowHeight="17500" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
+    <workbookView xWindow="4140" yWindow="7720" windowWidth="27960" windowHeight="17500" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="169">
   <si>
     <t>查找</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t>2. 两数相加</t>
+  </si>
+  <si>
+    <t>355. 设计推特</t>
   </si>
 </sst>
 </file>
@@ -927,7 +930,7 @@
   <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2641,7 +2644,18 @@
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D122" s="3"/>
+      <c r="A122">
+        <v>123</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C122" t="s">
+        <v>33</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D120" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}"/>
@@ -2760,6 +2774,8 @@
     <hyperlink ref="B116" r:id="rId112" xr:uid="{CCB20CB5-2063-F042-842E-3DF1AACB70D8}"/>
     <hyperlink ref="B117" r:id="rId113" xr:uid="{B1355D50-FC41-944A-BDE7-7A26E99DFB3D}"/>
     <hyperlink ref="B118" r:id="rId114" xr:uid="{ECF58827-D886-5544-8231-4C6D8F80D614}"/>
+    <hyperlink ref="B120" r:id="rId115" xr:uid="{91EAD357-0983-2341-AAD6-9260C1E44257}"/>
+    <hyperlink ref="B121" r:id="rId116" xr:uid="{E0061084-ACD3-064B-9444-D3F0BE40263D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add more problems of algorithm
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88126E5E-97DD-1C45-9BE0-6B337F1C5729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A170D1B5-C12A-EF43-B1C3-50D295D1A2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="500" windowWidth="27960" windowHeight="17500" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="177">
   <si>
     <t>查找</t>
   </si>
@@ -562,6 +562,12 @@
   </si>
   <si>
     <t>剑指 Offer 12. 矩阵中的路径</t>
+  </si>
+  <si>
+    <t>剑指 Offer 03. 数组中重复的数字</t>
+  </si>
+  <si>
+    <t>剑指 Offer 07. 重建二叉树</t>
   </si>
 </sst>
 </file>
@@ -948,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}">
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2745,6 +2751,34 @@
         <v>22</v>
       </c>
       <c r="D127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>129</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C128" t="s">
+        <v>22</v>
+      </c>
+      <c r="D128" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>130</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C129" t="s">
+        <v>50</v>
+      </c>
+      <c r="D129" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2873,6 +2907,8 @@
     <hyperlink ref="B125" r:id="rId120" xr:uid="{334C0DFE-1602-6F43-A61E-1AFA48662729}"/>
     <hyperlink ref="B126" r:id="rId121" xr:uid="{957ADB4E-5873-3540-ADE1-F5E34464DD77}"/>
     <hyperlink ref="B127" r:id="rId122" xr:uid="{F06CDBB6-A657-9E48-900A-CB3CFBBF68BF}"/>
+    <hyperlink ref="B128" r:id="rId123" xr:uid="{B4A0F597-BAA4-9242-8ADC-C779E154DABE}"/>
+    <hyperlink ref="B129" r:id="rId124" xr:uid="{3FC18B45-6686-DA45-A692-68D857A39AFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add some algorithms problems
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A170D1B5-C12A-EF43-B1C3-50D295D1A2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD924DC-F1D0-4342-92F0-BC252B36F394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="500" windowWidth="27960" windowHeight="17500" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
+    <workbookView xWindow="9120" yWindow="4100" windowWidth="27960" windowHeight="17500" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="201">
   <si>
     <t>查找</t>
   </si>
@@ -568,13 +568,85 @@
   </si>
   <si>
     <t>剑指 Offer 07. 重建二叉树</t>
+  </si>
+  <si>
+    <t>剑指 Offer 10- II. 青蛙跳台阶问题</t>
+  </si>
+  <si>
+    <t>剑指 Offer 14- I. 剪绳子</t>
+  </si>
+  <si>
+    <t>剑指 Offer 14- II. 剪绳子 II</t>
+  </si>
+  <si>
+    <t>剑指 Offer 15. 二进制中1的个数</t>
+  </si>
+  <si>
+    <t>剑指 Offer 17. 打印从1到最大的n位数</t>
+  </si>
+  <si>
+    <t>剑指 Offer 20. 表示数值的字符串</t>
+  </si>
+  <si>
+    <t>自动机</t>
+  </si>
+  <si>
+    <t>剑指 Offer 24. 反转链表</t>
+  </si>
+  <si>
+    <t>剑指 Offer 25. 合并两个排序的链表</t>
+  </si>
+  <si>
+    <t>剑指 Offer 28. 对称的二叉树</t>
+  </si>
+  <si>
+    <t>剑指 Offer 32 - II. 从上到下打印二叉树 II</t>
+  </si>
+  <si>
+    <t>剑指 Offer 32 - III. 从上到下打印二叉树 III</t>
+  </si>
+  <si>
+    <t>剑指 Offer 33. 二叉搜索树的后序遍历序列</t>
+  </si>
+  <si>
+    <t>剑指 Offer 34. 二叉树中和为某一值的路径</t>
+  </si>
+  <si>
+    <t>剑指 Offer 35. 复杂链表的复制</t>
+  </si>
+  <si>
+    <t>剑指 Offer 36. 二叉搜索树与双向链表</t>
+  </si>
+  <si>
+    <t>剑指 Offer 42. 连续子数组的最大和</t>
+  </si>
+  <si>
+    <t>剑指 Offer 44. 数字序列中某一位的数字</t>
+  </si>
+  <si>
+    <t>剑指 Offer 47. 礼物的最大价值</t>
+  </si>
+  <si>
+    <t>剑指 Offer 48. 最长不含重复字符的子字符串</t>
+  </si>
+  <si>
+    <t>剑指 Offer 49. 丑数</t>
+  </si>
+  <si>
+    <t>堆</t>
+  </si>
+  <si>
+    <t>剑指 Offer 50. 第一个只出现一次的字符</t>
+  </si>
+  <si>
+    <t>剑指 Offer 52. 两个链表的第一个公共节点</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -595,6 +667,14 @@
       <u/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -627,7 +707,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -639,6 +719,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -954,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}">
-  <dimension ref="A1:E129"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2725,6 +2806,7 @@
       <c r="D125" t="s">
         <v>27</v>
       </c>
+      <c r="E125" s="7"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126">
@@ -2780,6 +2862,328 @@
       </c>
       <c r="D129" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>131</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C130" t="s">
+        <v>14</v>
+      </c>
+      <c r="D130" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>132</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C131" t="s">
+        <v>14</v>
+      </c>
+      <c r="D131" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>133</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C132" t="s">
+        <v>14</v>
+      </c>
+      <c r="D132" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>134</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C133" t="s">
+        <v>166</v>
+      </c>
+      <c r="D133" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>135</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C134" t="s">
+        <v>22</v>
+      </c>
+      <c r="D134" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>136</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C135" t="s">
+        <v>183</v>
+      </c>
+      <c r="D135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>137</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C136" t="s">
+        <v>45</v>
+      </c>
+      <c r="D136" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>138</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C137" t="s">
+        <v>29</v>
+      </c>
+      <c r="D137" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>139</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C138" t="s">
+        <v>29</v>
+      </c>
+      <c r="D138" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>140</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C139" t="s">
+        <v>50</v>
+      </c>
+      <c r="D139" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>141</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C140" t="s">
+        <v>50</v>
+      </c>
+      <c r="D140" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>142</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C141" t="s">
+        <v>50</v>
+      </c>
+      <c r="D141" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>143</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C142" t="s">
+        <v>50</v>
+      </c>
+      <c r="D142" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>144</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C143" t="s">
+        <v>50</v>
+      </c>
+      <c r="D143" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>145</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C144" t="s">
+        <v>29</v>
+      </c>
+      <c r="D144" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>146</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C145" t="s">
+        <v>29</v>
+      </c>
+      <c r="D145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>147</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C146" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>148</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C147" t="s">
+        <v>3</v>
+      </c>
+      <c r="D147" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>149</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C148" t="s">
+        <v>14</v>
+      </c>
+      <c r="D148" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>150</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C149" t="s">
+        <v>45</v>
+      </c>
+      <c r="D149" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>151</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C150" t="s">
+        <v>198</v>
+      </c>
+      <c r="D150" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>152</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C151" t="s">
+        <v>61</v>
+      </c>
+      <c r="D151" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>153</v>
+      </c>
+      <c r="B152" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C152" t="s">
+        <v>29</v>
+      </c>
+      <c r="D152" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2834,81 +3238,99 @@
     <hyperlink ref="B54" r:id="rId47" display="https://leetcode.cn/problems/zhong-jian-er-cha-shu-lcof/" xr:uid="{78503987-1A08-8B49-88B5-DA0283091DA2}"/>
     <hyperlink ref="B55" r:id="rId48" display="https://leetcode.cn/problems/yong-liang-ge-zhan-shi-xian-dui-lie-lcof/" xr:uid="{B236A297-89FD-9949-8CA4-DAA89C1DE5D0}"/>
     <hyperlink ref="B56" r:id="rId49" display="https://leetcode.cn/problems/xuan-zhuan-shu-zu-de-zui-xiao-shu-zi-lcof/" xr:uid="{DF73D8E1-8572-3D4F-B8A5-550266891B79}"/>
-    <hyperlink ref="B57" r:id="rId50" display="https://leetcode.cn/problems/fei-bo-na-qi-shu-lie-lcof/" xr:uid="{C8D91180-3D90-7444-A782-63EB6EBE17D2}"/>
-    <hyperlink ref="B60" r:id="rId51" display="https://leetcode.cn/problems/diao-zheng-shu-zu-shun-xu-shi-qi-shu-wei-yu-ou-shu-qian-mian-lcof/" xr:uid="{443AA0AD-56B4-6740-A76C-FD22637011BD}"/>
-    <hyperlink ref="B61" r:id="rId52" display="https://leetcode.cn/problems/lian-biao-zhong-dao-shu-di-kge-jie-dian-lcof/" xr:uid="{56671026-2953-D644-AF44-997AE2F23AC5}"/>
-    <hyperlink ref="B62" r:id="rId53" display="https://leetcode.cn/problems/UHnkqh/" xr:uid="{0E5D1D0F-B375-9345-8B95-7E0194CB4E1E}"/>
-    <hyperlink ref="B63" r:id="rId54" display="https://leetcode.cn/problems/shu-de-zi-jie-gou-lcof/" xr:uid="{C71BADE5-9702-DA4B-8299-9790C751EB50}"/>
-    <hyperlink ref="B64" r:id="rId55" display="https://leetcode.cn/problems/er-cha-shu-de-jing-xiang-lcof/" xr:uid="{B3F80957-E27F-2542-A730-D0FA62BB3F8A}"/>
-    <hyperlink ref="B65" r:id="rId56" display="https://leetcode.cn/problems/spiral-matrix/" xr:uid="{CB478961-24CD-8544-A5EE-5E198C6560A6}"/>
-    <hyperlink ref="B66" r:id="rId57" display="https://leetcode.cn/problems/bao-han-minhan-shu-de-zhan-lcof/" xr:uid="{BB17BBD7-9053-6B4E-AC9E-7E5CFF54AA0C}"/>
-    <hyperlink ref="B67" r:id="rId58" display="https://leetcode.cn/problems/zhan-de-ya-ru-dan-chu-xu-lie-lcof/" xr:uid="{A2B658D4-24A6-4D49-8CB4-7D47FB72B277}"/>
-    <hyperlink ref="B68" r:id="rId59" display="https://leetcode.cn/problems/cong-shang-dao-xia-da-yin-er-cha-shu-lcof/" xr:uid="{B330BE06-FEE8-CC4C-8423-F177F0EADA52}"/>
-    <hyperlink ref="B69" r:id="rId60" display="https://leetcode.cn/problems/zi-fu-chuan-de-pai-lie-lcof/" xr:uid="{CE1EF55D-BAB1-E44F-A383-6ED6034540E9}"/>
-    <hyperlink ref="B70" r:id="rId61" display="https://leetcode.cn/problems/shu-zu-zhong-chu-xian-ci-shu-chao-guo-yi-ban-de-shu-zi-lcof/" xr:uid="{3BBAF4A0-0737-9B41-9774-E6005DEE76BB}"/>
-    <hyperlink ref="B71" r:id="rId62" display="https://leetcode.cn/problems/zui-xiao-de-kge-shu-lcof/" xr:uid="{0A86F043-35F2-FD46-B12C-9DB0DCCC24FA}"/>
-    <hyperlink ref="B72" r:id="rId63" display="https://leetcode.cn/problems/er-cha-shu-de-shen-du-lcof/" xr:uid="{6B0F3407-87C5-014A-946E-1686CE67CFE6}"/>
-    <hyperlink ref="B73" r:id="rId64" display="https://leetcode.cn/problems/ping-heng-er-cha-shu-lcof/" xr:uid="{08CF6D8D-00F4-5345-A4D0-EFEE6C340595}"/>
-    <hyperlink ref="B74" r:id="rId65" display="https://leetcode.cn/problems/first-missing-positive/" xr:uid="{90CAB2C8-E0CE-4C48-B6F3-45E918798F5D}"/>
-    <hyperlink ref="B75" r:id="rId66" display="https://leetcode.cn/problems/number-of-islands/" xr:uid="{020CC610-DD3F-8341-B586-EEEFE7999F1C}"/>
-    <hyperlink ref="B76" r:id="rId67" display="https://leetcode.cn/problems/maximum-number-of-balloons/" xr:uid="{431D9D90-5877-0146-A4A7-4988516D230D}"/>
-    <hyperlink ref="B77" r:id="rId68" display="https://leetcode.cn/problems/reverse-integer/" xr:uid="{E1196054-604B-904A-9E44-E0BA759E7AF4}"/>
-    <hyperlink ref="B78" r:id="rId69" display="https://leetcode.cn/problems/maximal-network-rank/" xr:uid="{DF9DD956-64F5-C443-874F-6207C6AADEEA}"/>
-    <hyperlink ref="B79" r:id="rId70" display="https://leetcode.cn/problems/subarray-sum-equals-k/" xr:uid="{94A9666E-B2B6-E541-9F3E-541A40EE5D81}"/>
-    <hyperlink ref="B80" r:id="rId71" display="https://leetcode.cn/problems/two-sum/" xr:uid="{24AD0B95-E868-2944-81FD-DA13933390A5}"/>
-    <hyperlink ref="B81" r:id="rId72" display="https://leetcode.cn/problems/shu-zu-zhong-de-ni-xu-dui-lcof/" xr:uid="{3B1B43D7-F39B-0740-8A3B-106889B3F55C}"/>
-    <hyperlink ref="B82" r:id="rId73" display="https://leetcode.cn/problems/trapping-rain-water/" xr:uid="{F38543FA-C8C5-964F-9DC3-494414764EE3}"/>
-    <hyperlink ref="B83" r:id="rId74" display="https://leetcode.cn/problems/symmetric-tree/" xr:uid="{E6488886-6415-9B4A-A977-5C770CB14B53}"/>
-    <hyperlink ref="B84" r:id="rId75" display="https://leetcode.cn/problems/reverse-nodes-in-k-group/" xr:uid="{DF0C3405-83A9-754E-9204-A6047B6DDA6F}"/>
-    <hyperlink ref="B85" r:id="rId76" display="https://leetcode.cn/problems/valid-parentheses/" xr:uid="{9D881CEE-41D6-514C-832F-414F716185D7}"/>
-    <hyperlink ref="B86" r:id="rId77" display="https://leetcode.cn/problems/subsets/" xr:uid="{9F3AB15D-49C0-CA44-95A5-20572ED9A8EB}"/>
-    <hyperlink ref="B87" r:id="rId78" display="https://leetcode.cn/problems/swap-nodes-in-pairs/" xr:uid="{D3499173-97D8-5743-847C-65FB05A3AF51}"/>
-    <hyperlink ref="B88" r:id="rId79" display="https://leetcode.cn/problems/combinations/" xr:uid="{843D4CEB-71C1-D146-BF8C-EC8C6DC9C762}"/>
-    <hyperlink ref="B89" r:id="rId80" display="https://leetcode.cn/problems/count-primes/" xr:uid="{8C083234-22AC-DC45-A1DE-A2B2A70F53D4}"/>
-    <hyperlink ref="B90" r:id="rId81" display="https://leetcode.cn/problems/permutations/" xr:uid="{13F47BF1-3464-784C-B4C5-B9FCD7A72D13}"/>
-    <hyperlink ref="B91" r:id="rId82" display="https://leetcode.cn/problems/flip-string-to-monotone-increasing/" xr:uid="{9D195D35-73B2-D845-A2F7-68E40FD9AB9E}"/>
-    <hyperlink ref="B92" r:id="rId83" display="https://leetcode.cn/problems/exam-room/" xr:uid="{3A7CA946-4DE4-A74F-84CF-7C2503CFCCCD}"/>
-    <hyperlink ref="B93" r:id="rId84" display="https://leetcode.cn/problems/top-k-frequent-elements/" xr:uid="{31CFF25F-B18E-724D-8816-1E4608805F5D}"/>
-    <hyperlink ref="B94" r:id="rId85" display="https://leetcode.cn/problems/longest-palindromic-substring/" xr:uid="{7771706A-C26B-E84B-842B-659991EC6C57}"/>
-    <hyperlink ref="B95" r:id="rId86" display="https://leetcode.cn/problems/linked-list-random-node/" xr:uid="{9FAB2F8C-E092-8B46-B83C-5C1A5B0C01F5}"/>
-    <hyperlink ref="B96" r:id="rId87" display="https://leetcode.cn/problems/random-pick-index/" xr:uid="{68D070D9-303E-E84C-8B7D-C45F6FF4B2EA}"/>
-    <hyperlink ref="B97" r:id="rId88" display="https://leetcode.cn/problems/find-all-numbers-disappeared-in-an-array/" xr:uid="{7025D6EA-FD5F-EE4F-8534-823000C421E3}"/>
-    <hyperlink ref="B98" r:id="rId89" display="https://leetcode.cn/problems/set-mismatch/" xr:uid="{B274C22A-7BDD-CA43-ABC6-7ABC3391C078}"/>
-    <hyperlink ref="B99" r:id="rId90" display="https://leetcode.cn/problems/k-diff-pairs-in-an-array/" xr:uid="{68840298-8BBA-9142-A3E1-D1FBC47A5609}"/>
-    <hyperlink ref="B100" r:id="rId91" display="https://leetcode.cn/problems/koko-eating-bananas/" xr:uid="{22440AE3-6894-064E-B0A5-2E1A9E747CFB}"/>
-    <hyperlink ref="B101" r:id="rId92" display="https://leetcode.cn/problems/capacity-to-ship-packages-within-d-days/" xr:uid="{17607A48-2F34-254C-A084-44096D04151D}"/>
-    <hyperlink ref="B102" r:id="rId93" display="https://leetcode.cn/problems/lowest-common-ancestor-of-a-binary-tree/" xr:uid="{ACE2428A-5660-F542-B49D-E0D3D07FFBEF}"/>
-    <hyperlink ref="B103" r:id="rId94" display="https://leetcode.cn/problems/merge-k-sorted-lists/" xr:uid="{3D98F6C7-6DBD-C645-AAB9-52BC44181441}"/>
-    <hyperlink ref="B104" r:id="rId95" display="https://leetcode.cn/problems/replace-words/" xr:uid="{6867BCFB-0A98-3145-B1EB-68EFAD95FF43}"/>
-    <hyperlink ref="B2" r:id="rId96" xr:uid="{D8D1BFC7-D21F-9445-A0AE-2AEFBC8B37DC}"/>
-    <hyperlink ref="B3" r:id="rId97" xr:uid="{02C23389-3DC3-0C47-9A06-426A57A1269B}"/>
-    <hyperlink ref="B11" r:id="rId98" xr:uid="{05341E8F-ACFD-BF46-AE0B-58FCBB9FEF94}"/>
-    <hyperlink ref="B59" r:id="rId99" display="https://leetcode.cn/problems/shan-chu-lian-biao-de-jie-dian-lcof/" xr:uid="{7A6A95E7-68D2-644F-8AB0-2973D2B03718}"/>
-    <hyperlink ref="B4" r:id="rId100" xr:uid="{5CE7CA3F-B194-524C-B3A3-DCEA556C18E5}"/>
-    <hyperlink ref="B58" r:id="rId101" display="https://leetcode.cn/problems/shu-zhi-de-zheng-shu-ci-fang-lcof/" xr:uid="{0E59664C-8F58-E148-9163-5ABF090805EF}"/>
-    <hyperlink ref="B105" r:id="rId102" xr:uid="{E7772A45-9B18-0E4E-A748-60A969953FD5}"/>
-    <hyperlink ref="B106" r:id="rId103" xr:uid="{D3F889B3-E0EE-7E49-ABF7-59204597F074}"/>
-    <hyperlink ref="B107" r:id="rId104" xr:uid="{9D7F37B6-FC78-2B4A-8A43-54B060B0AADD}"/>
-    <hyperlink ref="B108" r:id="rId105" xr:uid="{FFBCD4C1-FF57-A04F-A7D9-61D096AA07DD}"/>
-    <hyperlink ref="B109" r:id="rId106" xr:uid="{BCD20D20-E4BE-D648-8C0B-04A93AEEFD83}"/>
-    <hyperlink ref="B110" r:id="rId107" xr:uid="{756D06D0-1496-A947-A670-605935733755}"/>
-    <hyperlink ref="B111" r:id="rId108" xr:uid="{5A22A2F8-D88D-1947-8840-9950A6AA075C}"/>
-    <hyperlink ref="B112" r:id="rId109" xr:uid="{52C1604F-F5F3-9E40-B075-880C99BE21C6}"/>
-    <hyperlink ref="B10" r:id="rId110" xr:uid="{6F0EDE12-36C2-914E-BF54-2BF57000EAF1}"/>
-    <hyperlink ref="B114" r:id="rId111" xr:uid="{6039090F-359F-5448-927D-AFAC478A96FA}"/>
-    <hyperlink ref="B116" r:id="rId112" xr:uid="{CCB20CB5-2063-F042-842E-3DF1AACB70D8}"/>
-    <hyperlink ref="B117" r:id="rId113" xr:uid="{B1355D50-FC41-944A-BDE7-7A26E99DFB3D}"/>
-    <hyperlink ref="B118" r:id="rId114" xr:uid="{ECF58827-D886-5544-8231-4C6D8F80D614}"/>
-    <hyperlink ref="B120" r:id="rId115" xr:uid="{91EAD357-0983-2341-AAD6-9260C1E44257}"/>
-    <hyperlink ref="B121" r:id="rId116" xr:uid="{E0061084-ACD3-064B-9444-D3F0BE40263D}"/>
-    <hyperlink ref="B122" r:id="rId117" xr:uid="{37D5BACA-34F0-9C43-A193-4DC408F166F5}"/>
-    <hyperlink ref="B123" r:id="rId118" xr:uid="{EF058886-29D7-154D-8747-D0C653B38CFA}"/>
-    <hyperlink ref="B124" r:id="rId119" xr:uid="{8AF6FD98-81C0-6043-B90C-23757717E077}"/>
-    <hyperlink ref="B125" r:id="rId120" xr:uid="{334C0DFE-1602-6F43-A61E-1AFA48662729}"/>
-    <hyperlink ref="B126" r:id="rId121" xr:uid="{957ADB4E-5873-3540-ADE1-F5E34464DD77}"/>
-    <hyperlink ref="B127" r:id="rId122" xr:uid="{F06CDBB6-A657-9E48-900A-CB3CFBBF68BF}"/>
-    <hyperlink ref="B128" r:id="rId123" xr:uid="{B4A0F597-BAA4-9242-8ADC-C779E154DABE}"/>
-    <hyperlink ref="B129" r:id="rId124" xr:uid="{3FC18B45-6686-DA45-A692-68D857A39AFF}"/>
+    <hyperlink ref="B60" r:id="rId50" display="https://leetcode.cn/problems/diao-zheng-shu-zu-shun-xu-shi-qi-shu-wei-yu-ou-shu-qian-mian-lcof/" xr:uid="{443AA0AD-56B4-6740-A76C-FD22637011BD}"/>
+    <hyperlink ref="B61" r:id="rId51" display="https://leetcode.cn/problems/lian-biao-zhong-dao-shu-di-kge-jie-dian-lcof/" xr:uid="{56671026-2953-D644-AF44-997AE2F23AC5}"/>
+    <hyperlink ref="B62" r:id="rId52" display="https://leetcode.cn/problems/UHnkqh/" xr:uid="{0E5D1D0F-B375-9345-8B95-7E0194CB4E1E}"/>
+    <hyperlink ref="B63" r:id="rId53" display="https://leetcode.cn/problems/shu-de-zi-jie-gou-lcof/" xr:uid="{C71BADE5-9702-DA4B-8299-9790C751EB50}"/>
+    <hyperlink ref="B64" r:id="rId54" display="https://leetcode.cn/problems/er-cha-shu-de-jing-xiang-lcof/" xr:uid="{B3F80957-E27F-2542-A730-D0FA62BB3F8A}"/>
+    <hyperlink ref="B65" r:id="rId55" display="https://leetcode.cn/problems/spiral-matrix/" xr:uid="{CB478961-24CD-8544-A5EE-5E198C6560A6}"/>
+    <hyperlink ref="B66" r:id="rId56" display="https://leetcode.cn/problems/bao-han-minhan-shu-de-zhan-lcof/" xr:uid="{BB17BBD7-9053-6B4E-AC9E-7E5CFF54AA0C}"/>
+    <hyperlink ref="B67" r:id="rId57" display="https://leetcode.cn/problems/zhan-de-ya-ru-dan-chu-xu-lie-lcof/" xr:uid="{A2B658D4-24A6-4D49-8CB4-7D47FB72B277}"/>
+    <hyperlink ref="B68" r:id="rId58" display="https://leetcode.cn/problems/cong-shang-dao-xia-da-yin-er-cha-shu-lcof/" xr:uid="{B330BE06-FEE8-CC4C-8423-F177F0EADA52}"/>
+    <hyperlink ref="B69" r:id="rId59" display="https://leetcode.cn/problems/zi-fu-chuan-de-pai-lie-lcof/" xr:uid="{CE1EF55D-BAB1-E44F-A383-6ED6034540E9}"/>
+    <hyperlink ref="B70" r:id="rId60" display="https://leetcode.cn/problems/shu-zu-zhong-chu-xian-ci-shu-chao-guo-yi-ban-de-shu-zi-lcof/" xr:uid="{3BBAF4A0-0737-9B41-9774-E6005DEE76BB}"/>
+    <hyperlink ref="B71" r:id="rId61" display="https://leetcode.cn/problems/zui-xiao-de-kge-shu-lcof/" xr:uid="{0A86F043-35F2-FD46-B12C-9DB0DCCC24FA}"/>
+    <hyperlink ref="B72" r:id="rId62" display="https://leetcode.cn/problems/er-cha-shu-de-shen-du-lcof/" xr:uid="{6B0F3407-87C5-014A-946E-1686CE67CFE6}"/>
+    <hyperlink ref="B73" r:id="rId63" display="https://leetcode.cn/problems/ping-heng-er-cha-shu-lcof/" xr:uid="{08CF6D8D-00F4-5345-A4D0-EFEE6C340595}"/>
+    <hyperlink ref="B74" r:id="rId64" display="https://leetcode.cn/problems/first-missing-positive/" xr:uid="{90CAB2C8-E0CE-4C48-B6F3-45E918798F5D}"/>
+    <hyperlink ref="B75" r:id="rId65" display="https://leetcode.cn/problems/number-of-islands/" xr:uid="{020CC610-DD3F-8341-B586-EEEFE7999F1C}"/>
+    <hyperlink ref="B76" r:id="rId66" display="https://leetcode.cn/problems/maximum-number-of-balloons/" xr:uid="{431D9D90-5877-0146-A4A7-4988516D230D}"/>
+    <hyperlink ref="B77" r:id="rId67" display="https://leetcode.cn/problems/reverse-integer/" xr:uid="{E1196054-604B-904A-9E44-E0BA759E7AF4}"/>
+    <hyperlink ref="B78" r:id="rId68" display="https://leetcode.cn/problems/maximal-network-rank/" xr:uid="{DF9DD956-64F5-C443-874F-6207C6AADEEA}"/>
+    <hyperlink ref="B79" r:id="rId69" display="https://leetcode.cn/problems/subarray-sum-equals-k/" xr:uid="{94A9666E-B2B6-E541-9F3E-541A40EE5D81}"/>
+    <hyperlink ref="B80" r:id="rId70" display="https://leetcode.cn/problems/two-sum/" xr:uid="{24AD0B95-E868-2944-81FD-DA13933390A5}"/>
+    <hyperlink ref="B81" r:id="rId71" display="https://leetcode.cn/problems/shu-zu-zhong-de-ni-xu-dui-lcof/" xr:uid="{3B1B43D7-F39B-0740-8A3B-106889B3F55C}"/>
+    <hyperlink ref="B82" r:id="rId72" display="https://leetcode.cn/problems/trapping-rain-water/" xr:uid="{F38543FA-C8C5-964F-9DC3-494414764EE3}"/>
+    <hyperlink ref="B83" r:id="rId73" display="https://leetcode.cn/problems/symmetric-tree/" xr:uid="{E6488886-6415-9B4A-A977-5C770CB14B53}"/>
+    <hyperlink ref="B84" r:id="rId74" display="https://leetcode.cn/problems/reverse-nodes-in-k-group/" xr:uid="{DF0C3405-83A9-754E-9204-A6047B6DDA6F}"/>
+    <hyperlink ref="B85" r:id="rId75" display="https://leetcode.cn/problems/valid-parentheses/" xr:uid="{9D881CEE-41D6-514C-832F-414F716185D7}"/>
+    <hyperlink ref="B86" r:id="rId76" display="https://leetcode.cn/problems/subsets/" xr:uid="{9F3AB15D-49C0-CA44-95A5-20572ED9A8EB}"/>
+    <hyperlink ref="B87" r:id="rId77" display="https://leetcode.cn/problems/swap-nodes-in-pairs/" xr:uid="{D3499173-97D8-5743-847C-65FB05A3AF51}"/>
+    <hyperlink ref="B88" r:id="rId78" display="https://leetcode.cn/problems/combinations/" xr:uid="{843D4CEB-71C1-D146-BF8C-EC8C6DC9C762}"/>
+    <hyperlink ref="B89" r:id="rId79" display="https://leetcode.cn/problems/count-primes/" xr:uid="{8C083234-22AC-DC45-A1DE-A2B2A70F53D4}"/>
+    <hyperlink ref="B90" r:id="rId80" display="https://leetcode.cn/problems/permutations/" xr:uid="{13F47BF1-3464-784C-B4C5-B9FCD7A72D13}"/>
+    <hyperlink ref="B91" r:id="rId81" display="https://leetcode.cn/problems/flip-string-to-monotone-increasing/" xr:uid="{9D195D35-73B2-D845-A2F7-68E40FD9AB9E}"/>
+    <hyperlink ref="B92" r:id="rId82" display="https://leetcode.cn/problems/exam-room/" xr:uid="{3A7CA946-4DE4-A74F-84CF-7C2503CFCCCD}"/>
+    <hyperlink ref="B93" r:id="rId83" display="https://leetcode.cn/problems/top-k-frequent-elements/" xr:uid="{31CFF25F-B18E-724D-8816-1E4608805F5D}"/>
+    <hyperlink ref="B94" r:id="rId84" display="https://leetcode.cn/problems/longest-palindromic-substring/" xr:uid="{7771706A-C26B-E84B-842B-659991EC6C57}"/>
+    <hyperlink ref="B95" r:id="rId85" display="https://leetcode.cn/problems/linked-list-random-node/" xr:uid="{9FAB2F8C-E092-8B46-B83C-5C1A5B0C01F5}"/>
+    <hyperlink ref="B96" r:id="rId86" display="https://leetcode.cn/problems/random-pick-index/" xr:uid="{68D070D9-303E-E84C-8B7D-C45F6FF4B2EA}"/>
+    <hyperlink ref="B97" r:id="rId87" display="https://leetcode.cn/problems/find-all-numbers-disappeared-in-an-array/" xr:uid="{7025D6EA-FD5F-EE4F-8534-823000C421E3}"/>
+    <hyperlink ref="B98" r:id="rId88" display="https://leetcode.cn/problems/set-mismatch/" xr:uid="{B274C22A-7BDD-CA43-ABC6-7ABC3391C078}"/>
+    <hyperlink ref="B99" r:id="rId89" display="https://leetcode.cn/problems/k-diff-pairs-in-an-array/" xr:uid="{68840298-8BBA-9142-A3E1-D1FBC47A5609}"/>
+    <hyperlink ref="B100" r:id="rId90" display="https://leetcode.cn/problems/koko-eating-bananas/" xr:uid="{22440AE3-6894-064E-B0A5-2E1A9E747CFB}"/>
+    <hyperlink ref="B101" r:id="rId91" display="https://leetcode.cn/problems/capacity-to-ship-packages-within-d-days/" xr:uid="{17607A48-2F34-254C-A084-44096D04151D}"/>
+    <hyperlink ref="B102" r:id="rId92" display="https://leetcode.cn/problems/lowest-common-ancestor-of-a-binary-tree/" xr:uid="{ACE2428A-5660-F542-B49D-E0D3D07FFBEF}"/>
+    <hyperlink ref="B103" r:id="rId93" display="https://leetcode.cn/problems/merge-k-sorted-lists/" xr:uid="{3D98F6C7-6DBD-C645-AAB9-52BC44181441}"/>
+    <hyperlink ref="B104" r:id="rId94" display="https://leetcode.cn/problems/replace-words/" xr:uid="{6867BCFB-0A98-3145-B1EB-68EFAD95FF43}"/>
+    <hyperlink ref="B2" r:id="rId95" xr:uid="{D8D1BFC7-D21F-9445-A0AE-2AEFBC8B37DC}"/>
+    <hyperlink ref="B3" r:id="rId96" xr:uid="{02C23389-3DC3-0C47-9A06-426A57A1269B}"/>
+    <hyperlink ref="B11" r:id="rId97" xr:uid="{05341E8F-ACFD-BF46-AE0B-58FCBB9FEF94}"/>
+    <hyperlink ref="B59" r:id="rId98" display="https://leetcode.cn/problems/shan-chu-lian-biao-de-jie-dian-lcof/" xr:uid="{7A6A95E7-68D2-644F-8AB0-2973D2B03718}"/>
+    <hyperlink ref="B4" r:id="rId99" xr:uid="{5CE7CA3F-B194-524C-B3A3-DCEA556C18E5}"/>
+    <hyperlink ref="B58" r:id="rId100" display="https://leetcode.cn/problems/shu-zhi-de-zheng-shu-ci-fang-lcof/" xr:uid="{0E59664C-8F58-E148-9163-5ABF090805EF}"/>
+    <hyperlink ref="B105" r:id="rId101" xr:uid="{E7772A45-9B18-0E4E-A748-60A969953FD5}"/>
+    <hyperlink ref="B106" r:id="rId102" xr:uid="{D3F889B3-E0EE-7E49-ABF7-59204597F074}"/>
+    <hyperlink ref="B107" r:id="rId103" xr:uid="{9D7F37B6-FC78-2B4A-8A43-54B060B0AADD}"/>
+    <hyperlink ref="B108" r:id="rId104" xr:uid="{FFBCD4C1-FF57-A04F-A7D9-61D096AA07DD}"/>
+    <hyperlink ref="B109" r:id="rId105" xr:uid="{BCD20D20-E4BE-D648-8C0B-04A93AEEFD83}"/>
+    <hyperlink ref="B110" r:id="rId106" xr:uid="{756D06D0-1496-A947-A670-605935733755}"/>
+    <hyperlink ref="B111" r:id="rId107" xr:uid="{5A22A2F8-D88D-1947-8840-9950A6AA075C}"/>
+    <hyperlink ref="B112" r:id="rId108" xr:uid="{52C1604F-F5F3-9E40-B075-880C99BE21C6}"/>
+    <hyperlink ref="B10" r:id="rId109" xr:uid="{6F0EDE12-36C2-914E-BF54-2BF57000EAF1}"/>
+    <hyperlink ref="B114" r:id="rId110" xr:uid="{6039090F-359F-5448-927D-AFAC478A96FA}"/>
+    <hyperlink ref="B116" r:id="rId111" xr:uid="{CCB20CB5-2063-F042-842E-3DF1AACB70D8}"/>
+    <hyperlink ref="B117" r:id="rId112" xr:uid="{B1355D50-FC41-944A-BDE7-7A26E99DFB3D}"/>
+    <hyperlink ref="B118" r:id="rId113" xr:uid="{ECF58827-D886-5544-8231-4C6D8F80D614}"/>
+    <hyperlink ref="B120" r:id="rId114" xr:uid="{91EAD357-0983-2341-AAD6-9260C1E44257}"/>
+    <hyperlink ref="B121" r:id="rId115" xr:uid="{E0061084-ACD3-064B-9444-D3F0BE40263D}"/>
+    <hyperlink ref="B122" r:id="rId116" xr:uid="{37D5BACA-34F0-9C43-A193-4DC408F166F5}"/>
+    <hyperlink ref="B123" r:id="rId117" xr:uid="{EF058886-29D7-154D-8747-D0C653B38CFA}"/>
+    <hyperlink ref="B124" r:id="rId118" xr:uid="{8AF6FD98-81C0-6043-B90C-23757717E077}"/>
+    <hyperlink ref="B125" r:id="rId119" xr:uid="{334C0DFE-1602-6F43-A61E-1AFA48662729}"/>
+    <hyperlink ref="B126" r:id="rId120" xr:uid="{957ADB4E-5873-3540-ADE1-F5E34464DD77}"/>
+    <hyperlink ref="B127" r:id="rId121" xr:uid="{F06CDBB6-A657-9E48-900A-CB3CFBBF68BF}"/>
+    <hyperlink ref="B128" r:id="rId122" xr:uid="{B4A0F597-BAA4-9242-8ADC-C779E154DABE}"/>
+    <hyperlink ref="B129" r:id="rId123" xr:uid="{3FC18B45-6686-DA45-A692-68D857A39AFF}"/>
+    <hyperlink ref="B57" r:id="rId124" display="https://leetcode.cn/problems/fei-bo-na-qi-shu-lie-lcof/" xr:uid="{C8D91180-3D90-7444-A782-63EB6EBE17D2}"/>
+    <hyperlink ref="B130" r:id="rId125" xr:uid="{9985942E-FCF4-5F41-984A-291B7AFC711C}"/>
+    <hyperlink ref="B131" r:id="rId126" xr:uid="{B59ED4B8-AC0C-2D41-B315-684421C5FFCE}"/>
+    <hyperlink ref="B133" r:id="rId127" xr:uid="{2173DF10-7DA1-C04B-B479-9D2C8177C3A0}"/>
+    <hyperlink ref="B134" r:id="rId128" xr:uid="{1182C11A-BF02-1D46-B6B8-87CDFF86E546}"/>
+    <hyperlink ref="B137" r:id="rId129" xr:uid="{1D6C2D37-E1E8-824B-A932-8241583E8E79}"/>
+    <hyperlink ref="B138" r:id="rId130" xr:uid="{5E92F064-7E83-B54A-BA56-910B637EB6C5}"/>
+    <hyperlink ref="B139" r:id="rId131" xr:uid="{AE73E400-5DF0-2F47-A734-B9CF8E0754DA}"/>
+    <hyperlink ref="B140" r:id="rId132" xr:uid="{C59B6532-9A3D-314D-B183-C3C0C742A507}"/>
+    <hyperlink ref="B141" r:id="rId133" xr:uid="{458C7376-6AE2-4C47-B361-1D0C795D50FD}"/>
+    <hyperlink ref="B143" r:id="rId134" xr:uid="{2C546845-52BB-D142-B6F7-9FE7BEF5817F}"/>
+    <hyperlink ref="B144" r:id="rId135" xr:uid="{7400F6F1-93E5-8B4D-8204-1B0EF5A86FAF}"/>
+    <hyperlink ref="B145" r:id="rId136" xr:uid="{863045FD-4CD8-CA48-AD93-8A9F81F098FC}"/>
+    <hyperlink ref="B146" r:id="rId137" xr:uid="{905C8D8C-706A-CD45-95AC-5AABE95A0E55}"/>
+    <hyperlink ref="B148" r:id="rId138" xr:uid="{5752E351-D6AB-3044-B467-EDF2AB64AB69}"/>
+    <hyperlink ref="B149" r:id="rId139" xr:uid="{1456E733-B9E1-FF41-A7FE-CE4DCB4B2CF4}"/>
+    <hyperlink ref="B150" r:id="rId140" xr:uid="{E01530A4-8E45-214E-B804-70E6E716F1D5}"/>
+    <hyperlink ref="B151" r:id="rId141" xr:uid="{32D5F016-4FF7-2A4D-A9D4-388ED3BFF442}"/>
+    <hyperlink ref="B152" r:id="rId142" xr:uid="{629D218F-BDD7-FA46-B861-F1363D4AAD1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add some algorithm problems and fix some 'vet' issues
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD924DC-F1D0-4342-92F0-BC252B36F394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17934DFB-BCEE-2C4E-AC94-2161582A2727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9120" yWindow="4100" windowWidth="27960" windowHeight="17500" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="204">
   <si>
     <t>查找</t>
   </si>
@@ -640,6 +640,15 @@
   </si>
   <si>
     <t>剑指 Offer 52. 两个链表的第一个公共节点</t>
+  </si>
+  <si>
+    <t>剑指 Offer 53 - I. 在排序数组中查找数字 I</t>
+  </si>
+  <si>
+    <t>剑指 Offer 53 - II. 0～n-1中缺失的数字</t>
+  </si>
+  <si>
+    <t>剑指 Offer 54. 二叉搜索树的第k大节点</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}">
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E155"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="E140" sqref="E140"/>
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3183,6 +3192,48 @@
         <v>29</v>
       </c>
       <c r="D152" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>154</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C153" t="s">
+        <v>3</v>
+      </c>
+      <c r="D153" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>155</v>
+      </c>
+      <c r="B154" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C154" t="s">
+        <v>22</v>
+      </c>
+      <c r="D154" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>156</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="C155" t="s">
+        <v>50</v>
+      </c>
+      <c r="D155" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3331,6 +3382,8 @@
     <hyperlink ref="B150" r:id="rId140" xr:uid="{E01530A4-8E45-214E-B804-70E6E716F1D5}"/>
     <hyperlink ref="B151" r:id="rId141" xr:uid="{32D5F016-4FF7-2A4D-A9D4-388ED3BFF442}"/>
     <hyperlink ref="B152" r:id="rId142" xr:uid="{629D218F-BDD7-FA46-B861-F1363D4AAD1E}"/>
+    <hyperlink ref="B153" r:id="rId143" xr:uid="{13DD5FF6-9802-B94E-AF31-B5A6C67B7B35}"/>
+    <hyperlink ref="B154" r:id="rId144" xr:uid="{17DFCABC-0FDF-E64F-9372-9815921AE262}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add more algorithm problems and fix vet issues.
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454045FE-D3F2-0D42-821D-34C95E469A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4E5C63-79D1-734B-AD25-C83FA89DCB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9120" yWindow="4100" windowWidth="27960" windowHeight="17500" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="205">
   <si>
     <t>查找</t>
   </si>
@@ -649,6 +649,9 @@
   </si>
   <si>
     <t>剑指 Offer 54. 二叉搜索树的第k大节点</t>
+  </si>
+  <si>
+    <t>剑指 Offer 56 - I. 数组中数字出现的次数</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}">
-  <dimension ref="A1:E155"/>
+  <dimension ref="A1:E156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="E135" sqref="E135"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="E145" sqref="E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3235,6 +3238,20 @@
       </c>
       <c r="D155" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>157</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C156" t="s">
+        <v>50</v>
+      </c>
+      <c r="D156" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3385,6 +3402,7 @@
     <hyperlink ref="B153" r:id="rId143" xr:uid="{13DD5FF6-9802-B94E-AF31-B5A6C67B7B35}"/>
     <hyperlink ref="B154" r:id="rId144" xr:uid="{17DFCABC-0FDF-E64F-9372-9815921AE262}"/>
     <hyperlink ref="B155" r:id="rId145" xr:uid="{08A04A15-E1A9-9A48-9CA4-F5A749BBA37E}"/>
+    <hyperlink ref="B156" r:id="rId146" xr:uid="{04B5D6DF-563C-2A47-8930-CE1E02372723}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Add a algorithm problem with double points solution.
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4E5C63-79D1-734B-AD25-C83FA89DCB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B077C8-28F2-3C4C-B10D-9913E587761B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9120" yWindow="4100" windowWidth="27960" windowHeight="17500" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
+    <workbookView xWindow="840" yWindow="500" windowWidth="27960" windowHeight="17500" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="206">
   <si>
     <t>查找</t>
   </si>
@@ -652,6 +652,9 @@
   </si>
   <si>
     <t>剑指 Offer 56 - I. 数组中数字出现的次数</t>
+  </si>
+  <si>
+    <t>剑指 Offer 57 - II. 和为s的连续正数序列</t>
   </si>
 </sst>
 </file>
@@ -1047,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}">
-  <dimension ref="A1:E156"/>
+  <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="E145" sqref="E145"/>
+      <selection activeCell="D144" sqref="D144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3252,6 +3255,20 @@
       </c>
       <c r="D156" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>158</v>
+      </c>
+      <c r="B157" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C157" t="s">
+        <v>172</v>
+      </c>
+      <c r="D157" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3403,6 +3420,7 @@
     <hyperlink ref="B154" r:id="rId144" xr:uid="{17DFCABC-0FDF-E64F-9372-9815921AE262}"/>
     <hyperlink ref="B155" r:id="rId145" xr:uid="{08A04A15-E1A9-9A48-9CA4-F5A749BBA37E}"/>
     <hyperlink ref="B156" r:id="rId146" xr:uid="{04B5D6DF-563C-2A47-8930-CE1E02372723}"/>
+    <hyperlink ref="B157" r:id="rId147" xr:uid="{BD63DEE7-18E1-194D-AFE7-646D10074556}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add some algorithm problems.
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0968C439-6EB6-E04A-8654-E6B4C306C901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB37191-6243-9B42-9411-4EC1E76FE01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="500" windowWidth="37560" windowHeight="21100" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="210">
   <si>
     <t>查找</t>
   </si>
@@ -661,6 +661,12 @@
   </si>
   <si>
     <t>剑指 Offer 58 - II. 左旋转字符串</t>
+  </si>
+  <si>
+    <t>剑指 Offer 60. n个骰子的点数</t>
+  </si>
+  <si>
+    <t>剑指 Offer 62. 圆圈中最后剩下的数字</t>
   </si>
 </sst>
 </file>
@@ -1056,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}">
-  <dimension ref="A1:E159"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="E157" sqref="E157"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3302,6 +3308,34 @@
         <v>45</v>
       </c>
       <c r="D159" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>161</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C160" t="s">
+        <v>14</v>
+      </c>
+      <c r="D160" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>162</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C161" t="s">
+        <v>85</v>
+      </c>
+      <c r="D161" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3457,6 +3491,8 @@
     <hyperlink ref="B157" r:id="rId147" xr:uid="{BD63DEE7-18E1-194D-AFE7-646D10074556}"/>
     <hyperlink ref="B158" r:id="rId148" xr:uid="{652521D9-EB65-3440-B1FA-20EF5898C39E}"/>
     <hyperlink ref="B159" r:id="rId149" xr:uid="{30238197-1683-2A45-B098-368DD23F6F98}"/>
+    <hyperlink ref="B160" r:id="rId150" xr:uid="{4AAB76CC-9D82-974B-AC5B-CDCE04E13889}"/>
+    <hyperlink ref="B161" r:id="rId151" xr:uid="{EC2339D2-6390-494F-A703-DF9DBE087EBC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add some algorithm problems about dp and array.
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB37191-6243-9B42-9411-4EC1E76FE01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8843CCAC-4A3E-3340-B5B4-5E1A587CBE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="500" windowWidth="37560" windowHeight="21100" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
+    <workbookView xWindow="840" yWindow="500" windowWidth="18780" windowHeight="21100" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="215">
   <si>
     <t>查找</t>
   </si>
@@ -667,6 +667,21 @@
   </si>
   <si>
     <t>剑指 Offer 62. 圆圈中最后剩下的数字</t>
+  </si>
+  <si>
+    <t>剑指 Offer 63. 股票的最大利润</t>
+  </si>
+  <si>
+    <t>面试题13. 机器人的运动范围</t>
+  </si>
+  <si>
+    <t>面试题45. 把数组排成最小的数</t>
+  </si>
+  <si>
+    <t>面试题59 - II. 队列的最大值</t>
+  </si>
+  <si>
+    <t>面试题61. 扑克牌中的顺子</t>
   </si>
 </sst>
 </file>
@@ -1062,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C169" sqref="C169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3336,6 +3351,76 @@
         <v>85</v>
       </c>
       <c r="D161" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>163</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C162" t="s">
+        <v>14</v>
+      </c>
+      <c r="D162" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>164</v>
+      </c>
+      <c r="B163" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C163" t="s">
+        <v>35</v>
+      </c>
+      <c r="D163" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>165</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C164" t="s">
+        <v>45</v>
+      </c>
+      <c r="D164" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>166</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C165" t="s">
+        <v>35</v>
+      </c>
+      <c r="D165" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>167</v>
+      </c>
+      <c r="B166" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C166" t="s">
+        <v>22</v>
+      </c>
+      <c r="D166" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3493,6 +3578,10 @@
     <hyperlink ref="B159" r:id="rId149" xr:uid="{30238197-1683-2A45-B098-368DD23F6F98}"/>
     <hyperlink ref="B160" r:id="rId150" xr:uid="{4AAB76CC-9D82-974B-AC5B-CDCE04E13889}"/>
     <hyperlink ref="B161" r:id="rId151" xr:uid="{EC2339D2-6390-494F-A703-DF9DBE087EBC}"/>
+    <hyperlink ref="B162" r:id="rId152" xr:uid="{2336C014-EE0D-7447-917E-C1DAA576C1E3}"/>
+    <hyperlink ref="B163" r:id="rId153" xr:uid="{3FA1506C-60D5-B544-9CDC-AFAFB8445F98}"/>
+    <hyperlink ref="B164" r:id="rId154" xr:uid="{E7E3CA6A-8508-C749-ADCE-B508EB0F9BBC}"/>
+    <hyperlink ref="B165" r:id="rId155" xr:uid="{7CA18804-E3E9-CF4D-8671-B6B700ECF835}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add a algorithm problem about string and finite automation
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8843CCAC-4A3E-3340-B5B4-5E1A587CBE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76F8932-026B-5A43-8D75-7488551F7E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="500" windowWidth="18780" windowHeight="21100" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="216">
   <si>
     <t>查找</t>
   </si>
@@ -682,6 +682,9 @@
   </si>
   <si>
     <t>面试题61. 扑克牌中的顺子</t>
+  </si>
+  <si>
+    <t>面试题67. 把字符串转换成整数</t>
   </si>
 </sst>
 </file>
@@ -1077,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C169" sqref="C169"/>
+      <selection activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3422,6 +3425,20 @@
       </c>
       <c r="D166" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>168</v>
+      </c>
+      <c r="B167" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C167" t="s">
+        <v>45</v>
+      </c>
+      <c r="D167" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3582,6 +3599,8 @@
     <hyperlink ref="B163" r:id="rId153" xr:uid="{3FA1506C-60D5-B544-9CDC-AFAFB8445F98}"/>
     <hyperlink ref="B164" r:id="rId154" xr:uid="{E7E3CA6A-8508-C749-ADCE-B508EB0F9BBC}"/>
     <hyperlink ref="B165" r:id="rId155" xr:uid="{7CA18804-E3E9-CF4D-8671-B6B700ECF835}"/>
+    <hyperlink ref="B166" r:id="rId156" xr:uid="{31A0F274-1A4C-7B4E-8442-01F587F9D601}"/>
+    <hyperlink ref="B167" r:id="rId157" xr:uid="{9200D37B-03CB-7947-955E-D9B241DA796D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add a algorithm problem about binary tree.
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76F8932-026B-5A43-8D75-7488551F7E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B54C049-C58D-D54D-9645-691FAF8C8DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="500" windowWidth="18780" windowHeight="21100" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="217">
   <si>
     <t>查找</t>
   </si>
@@ -685,6 +685,9 @@
   </si>
   <si>
     <t>面试题67. 把字符串转换成整数</t>
+  </si>
+  <si>
+    <t>剑指 Offer 68 - II. 二叉树的最近公共祖先</t>
   </si>
 </sst>
 </file>
@@ -1080,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="D167" sqref="D167"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3438,6 +3441,20 @@
         <v>45</v>
       </c>
       <c r="D167" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>169</v>
+      </c>
+      <c r="B168" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C168" t="s">
+        <v>50</v>
+      </c>
+      <c r="D168" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add a algorithm problem about string.
</commit_message>
<xml_diff>
--- a/algorithms/data_structure_and_algorithm.xlsx
+++ b/algorithms/data_structure_and_algorithm.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go-opt/algorithms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luojun/git/go/go-opt/algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B54C049-C58D-D54D-9645-691FAF8C8DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C424269D-B886-C04B-8D62-82E666599713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="500" windowWidth="18780" windowHeight="21100" xr2:uid="{B1EBE0FD-41CF-6C45-BA71-A6F356EE76A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="218">
   <si>
     <t>查找</t>
   </si>
@@ -688,6 +688,9 @@
   </si>
   <si>
     <t>剑指 Offer 68 - II. 二叉树的最近公共祖先</t>
+  </si>
+  <si>
+    <t>1625. 执行操作后字典序最小的字符串</t>
   </si>
 </sst>
 </file>
@@ -1083,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595610DC-C2FF-1D44-B87B-FBFFF144A60B}">
-  <dimension ref="A1:E168"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C170" sqref="C170"/>
+      <selection activeCell="E147" sqref="E147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3455,6 +3458,20 @@
         <v>50</v>
       </c>
       <c r="D168" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>170</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C169" t="s">
+        <v>45</v>
+      </c>
+      <c r="D169" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3618,6 +3635,7 @@
     <hyperlink ref="B165" r:id="rId155" xr:uid="{7CA18804-E3E9-CF4D-8671-B6B700ECF835}"/>
     <hyperlink ref="B166" r:id="rId156" xr:uid="{31A0F274-1A4C-7B4E-8442-01F587F9D601}"/>
     <hyperlink ref="B167" r:id="rId157" xr:uid="{9200D37B-03CB-7947-955E-D9B241DA796D}"/>
+    <hyperlink ref="B169" r:id="rId158" xr:uid="{6E27E84F-25F3-0B4A-A389-32BED16AE1AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>